<commit_message>
Teste de busca data+sensação termica
</commit_message>
<xml_diff>
--- a/Ciencias_de_dados/Relatório.xlsx
+++ b/Ciencias_de_dados/Relatório.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E105"/>
+  <dimension ref="A1:E109"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -466,17 +466,17 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>4,99</t>
+          <t>4,86</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>17:33</t>
+          <t>01:14</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t xml:space="preserve"> quarta-feira, 3 de maio de 2023 </t>
+          <t xml:space="preserve"> quarta-feira, 14 de junho de 2023 </t>
         </is>
       </c>
     </row>
@@ -491,17 +491,17 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>5,51</t>
+          <t>5,24</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>17:33</t>
+          <t>01:14</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t xml:space="preserve"> quarta-feira, 3 de maio de 2023 </t>
+          <t xml:space="preserve"> quarta-feira, 14 de junho de 2023 </t>
         </is>
       </c>
     </row>
@@ -516,17 +516,17 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>0,037</t>
+          <t>0,035</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>17:33</t>
+          <t>01:14</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t xml:space="preserve"> quarta-feira, 3 de maio de 2023 </t>
+          <t xml:space="preserve"> quarta-feira, 14 de junho de 2023 </t>
         </is>
       </c>
     </row>
@@ -541,17 +541,17 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>0,72</t>
+          <t>0,68</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>17:33</t>
+          <t>01:14</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t xml:space="preserve"> quarta-feira, 3 de maio de 2023 </t>
+          <t xml:space="preserve"> quarta-feira, 14 de junho de 2023 </t>
         </is>
       </c>
     </row>
@@ -571,12 +571,12 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>16:59</t>
+          <t>17:33</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t xml:space="preserve"> domingo, 30 de abril de 2023 </t>
+          <t xml:space="preserve"> quarta-feira, 3 de maio de 2023 </t>
         </is>
       </c>
     </row>
@@ -591,17 +591,17 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>5,50</t>
+          <t>5,51</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>16:59</t>
+          <t>17:33</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t xml:space="preserve"> domingo, 30 de abril de 2023 </t>
+          <t xml:space="preserve"> quarta-feira, 3 de maio de 2023 </t>
         </is>
       </c>
     </row>
@@ -621,12 +621,12 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>16:59</t>
+          <t>17:33</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t xml:space="preserve"> domingo, 30 de abril de 2023 </t>
+          <t xml:space="preserve"> quarta-feira, 3 de maio de 2023 </t>
         </is>
       </c>
     </row>
@@ -646,12 +646,12 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>16:59</t>
+          <t>17:33</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t xml:space="preserve"> domingo, 30 de abril de 2023 </t>
+          <t xml:space="preserve"> quarta-feira, 3 de maio de 2023 </t>
         </is>
       </c>
     </row>
@@ -666,17 +666,17 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>5,08</t>
+          <t>4,99</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>19:27</t>
+          <t>16:59</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t xml:space="preserve"> quarta-feira, 19 de abril de 2023 </t>
+          <t xml:space="preserve"> domingo, 30 de abril de 2023 </t>
         </is>
       </c>
     </row>
@@ -691,17 +691,17 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>5,56</t>
+          <t>5,50</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>19:27</t>
+          <t>16:59</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t xml:space="preserve"> quarta-feira, 19 de abril de 2023 </t>
+          <t xml:space="preserve"> domingo, 30 de abril de 2023 </t>
         </is>
       </c>
     </row>
@@ -716,17 +716,17 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>0,038</t>
+          <t>0,037</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>19:27</t>
+          <t>16:59</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t xml:space="preserve"> quarta-feira, 19 de abril de 2023 </t>
+          <t xml:space="preserve"> domingo, 30 de abril de 2023 </t>
         </is>
       </c>
     </row>
@@ -741,17 +741,17 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>0,74</t>
+          <t>0,72</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>19:27</t>
+          <t>16:59</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t xml:space="preserve"> quarta-feira, 19 de abril de 2023 </t>
+          <t xml:space="preserve"> domingo, 30 de abril de 2023 </t>
         </is>
       </c>
     </row>
@@ -771,7 +771,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>19:16</t>
+          <t>19:27</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -796,7 +796,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>19:16</t>
+          <t>19:27</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -821,7 +821,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>19:16</t>
+          <t>19:27</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -846,7 +846,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>19:16</t>
+          <t>19:27</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -871,7 +871,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>19:08</t>
+          <t>19:16</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -896,7 +896,7 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>19:08</t>
+          <t>19:16</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -921,7 +921,7 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>19:08</t>
+          <t>19:16</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -946,7 +946,7 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>19:08</t>
+          <t>19:16</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -966,17 +966,17 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>4,91</t>
+          <t>5,08</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>12:31</t>
+          <t>19:08</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t xml:space="preserve"> sábado, 15 de abril de 2023 </t>
+          <t xml:space="preserve"> quarta-feira, 19 de abril de 2023 </t>
         </is>
       </c>
     </row>
@@ -991,17 +991,17 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>5,45</t>
+          <t>5,56</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>12:31</t>
+          <t>19:08</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t xml:space="preserve"> sábado, 15 de abril de 2023 </t>
+          <t xml:space="preserve"> quarta-feira, 19 de abril de 2023 </t>
         </is>
       </c>
     </row>
@@ -1016,17 +1016,17 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>0,037</t>
+          <t>0,038</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>12:31</t>
+          <t>19:08</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t xml:space="preserve"> sábado, 15 de abril de 2023 </t>
+          <t xml:space="preserve"> quarta-feira, 19 de abril de 2023 </t>
         </is>
       </c>
     </row>
@@ -1041,17 +1041,17 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>0,71</t>
+          <t>0,74</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>12:31</t>
+          <t>19:08</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t xml:space="preserve"> sábado, 15 de abril de 2023 </t>
+          <t xml:space="preserve"> quarta-feira, 19 de abril de 2023 </t>
         </is>
       </c>
     </row>
@@ -1071,7 +1071,7 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>12:29</t>
+          <t>12:31</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
@@ -1096,7 +1096,7 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>12:29</t>
+          <t>12:31</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
@@ -1121,7 +1121,7 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>12:29</t>
+          <t>12:31</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
@@ -1146,7 +1146,7 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>12:29</t>
+          <t>12:31</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
@@ -1166,17 +1166,17 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>4,93</t>
+          <t>4,91</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>18:31</t>
+          <t>12:29</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t xml:space="preserve"> quinta-feira, 13 de abril de 2023 </t>
+          <t xml:space="preserve"> sábado, 15 de abril de 2023 </t>
         </is>
       </c>
     </row>
@@ -1191,17 +1191,17 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>5,44</t>
+          <t>5,45</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>18:31</t>
+          <t>12:29</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t xml:space="preserve"> quinta-feira, 13 de abril de 2023 </t>
+          <t xml:space="preserve"> sábado, 15 de abril de 2023 </t>
         </is>
       </c>
     </row>
@@ -1221,12 +1221,12 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>18:31</t>
+          <t>12:29</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t xml:space="preserve"> quinta-feira, 13 de abril de 2023 </t>
+          <t xml:space="preserve"> sábado, 15 de abril de 2023 </t>
         </is>
       </c>
     </row>
@@ -1241,17 +1241,17 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>0,72</t>
+          <t>0,71</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>18:31</t>
+          <t>12:29</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t xml:space="preserve"> quinta-feira, 13 de abril de 2023 </t>
+          <t xml:space="preserve"> sábado, 15 de abril de 2023 </t>
         </is>
       </c>
     </row>
@@ -1271,7 +1271,7 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>17:50</t>
+          <t>18:31</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
@@ -1291,12 +1291,12 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>5,45</t>
+          <t>5,44</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>17:50</t>
+          <t>18:31</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
@@ -1321,7 +1321,7 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>17:50</t>
+          <t>18:31</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
@@ -1346,7 +1346,7 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>17:50</t>
+          <t>18:31</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
@@ -1371,7 +1371,7 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>17:48</t>
+          <t>17:50</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
@@ -1396,7 +1396,7 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>17:48</t>
+          <t>17:50</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
@@ -1421,7 +1421,7 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>17:48</t>
+          <t>17:50</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
@@ -1446,7 +1446,7 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>17:48</t>
+          <t>17:50</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
@@ -1471,7 +1471,7 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>17:47</t>
+          <t>17:48</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
@@ -1491,12 +1491,12 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>5,44</t>
+          <t>5,45</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>17:47</t>
+          <t>17:48</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
@@ -1521,7 +1521,7 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>17:47</t>
+          <t>17:48</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
@@ -1546,7 +1546,7 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>17:47</t>
+          <t>17:48</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
@@ -1571,7 +1571,7 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>17:45</t>
+          <t>17:47</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
@@ -1596,7 +1596,7 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>17:45</t>
+          <t>17:47</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
@@ -1621,7 +1621,7 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>17:45</t>
+          <t>17:47</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
@@ -1646,7 +1646,7 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>17:45</t>
+          <t>17:47</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
@@ -1671,7 +1671,7 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>17:38</t>
+          <t>17:45</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
@@ -1691,12 +1691,12 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>5,45</t>
+          <t>5,44</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>17:38</t>
+          <t>17:45</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
@@ -1721,7 +1721,7 @@
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>17:38</t>
+          <t>17:45</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
@@ -1746,7 +1746,7 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>17:38</t>
+          <t>17:45</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
@@ -1771,7 +1771,7 @@
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>17:32</t>
+          <t>17:38</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
@@ -1791,12 +1791,12 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>5,44</t>
+          <t>5,45</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>17:32</t>
+          <t>17:38</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
@@ -1821,7 +1821,7 @@
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>17:32</t>
+          <t>17:38</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
@@ -1846,7 +1846,7 @@
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>17:32</t>
+          <t>17:38</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
@@ -1871,7 +1871,7 @@
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>17:29</t>
+          <t>17:32</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
@@ -1896,7 +1896,7 @@
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>17:29</t>
+          <t>17:32</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
@@ -1921,7 +1921,7 @@
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>17:29</t>
+          <t>17:32</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
@@ -1946,7 +1946,7 @@
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>17:29</t>
+          <t>17:32</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
@@ -1966,17 +1966,17 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>5,03</t>
+          <t>4,93</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>22:32</t>
+          <t>17:29</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t xml:space="preserve"> quarta-feira, 5 de abril de 2023 </t>
+          <t xml:space="preserve"> quinta-feira, 13 de abril de 2023 </t>
         </is>
       </c>
     </row>
@@ -1991,17 +1991,17 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>5,48</t>
+          <t>5,44</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>22:32</t>
+          <t>17:29</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t xml:space="preserve"> quarta-feira, 5 de abril de 2023 </t>
+          <t xml:space="preserve"> quinta-feira, 13 de abril de 2023 </t>
         </is>
       </c>
     </row>
@@ -2016,17 +2016,17 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>0,038</t>
+          <t>0,037</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>22:32</t>
+          <t>17:29</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t xml:space="preserve"> quarta-feira, 5 de abril de 2023 </t>
+          <t xml:space="preserve"> quinta-feira, 13 de abril de 2023 </t>
         </is>
       </c>
     </row>
@@ -2041,17 +2041,17 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>0,73</t>
+          <t>0,72</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>22:32</t>
+          <t>17:29</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t xml:space="preserve"> quarta-feira, 5 de abril de 2023 </t>
+          <t xml:space="preserve"> quinta-feira, 13 de abril de 2023 </t>
         </is>
       </c>
     </row>
@@ -2071,7 +2071,7 @@
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>21:21</t>
+          <t>22:32</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
@@ -2091,12 +2091,12 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>5,49</t>
+          <t>5,48</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>21:21</t>
+          <t>22:32</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
@@ -2121,7 +2121,7 @@
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>21:21</t>
+          <t>22:32</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
@@ -2146,7 +2146,7 @@
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>21:21</t>
+          <t>22:32</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
@@ -2171,7 +2171,7 @@
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>21:20</t>
+          <t>21:21</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
@@ -2196,7 +2196,7 @@
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>21:20</t>
+          <t>21:21</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
@@ -2221,7 +2221,7 @@
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>21:20</t>
+          <t>21:21</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
@@ -2246,7 +2246,7 @@
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>21:20</t>
+          <t>21:21</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
@@ -2366,17 +2366,17 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>4,93</t>
+          <t>5,03</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>17:38</t>
+          <t>21:20</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t xml:space="preserve"> quinta-feira, 13 de abril de 2023 </t>
+          <t xml:space="preserve"> quarta-feira, 5 de abril de 2023 </t>
         </is>
       </c>
     </row>
@@ -2391,17 +2391,17 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>5,45</t>
+          <t>5,49</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>17:38</t>
+          <t>21:20</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t xml:space="preserve"> quinta-feira, 13 de abril de 2023 </t>
+          <t xml:space="preserve"> quarta-feira, 5 de abril de 2023 </t>
         </is>
       </c>
     </row>
@@ -2416,17 +2416,17 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>0,037</t>
+          <t>0,038</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>17:38</t>
+          <t>21:20</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t xml:space="preserve"> quinta-feira, 13 de abril de 2023 </t>
+          <t xml:space="preserve"> quarta-feira, 5 de abril de 2023 </t>
         </is>
       </c>
     </row>
@@ -2441,17 +2441,17 @@
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>0,72</t>
+          <t>0,73</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>17:38</t>
+          <t>21:20</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t xml:space="preserve"> quinta-feira, 13 de abril de 2023 </t>
+          <t xml:space="preserve"> quarta-feira, 5 de abril de 2023 </t>
         </is>
       </c>
     </row>
@@ -2471,7 +2471,7 @@
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>17:32</t>
+          <t>17:38</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
@@ -2491,12 +2491,12 @@
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>5,44</t>
+          <t>5,45</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>17:32</t>
+          <t>17:38</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
@@ -2521,7 +2521,7 @@
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>17:32</t>
+          <t>17:38</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
@@ -2546,7 +2546,7 @@
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>17:32</t>
+          <t>17:38</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
@@ -2571,7 +2571,7 @@
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>17:29</t>
+          <t>17:32</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
@@ -2596,7 +2596,7 @@
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>17:29</t>
+          <t>17:32</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
@@ -2621,7 +2621,7 @@
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>17:29</t>
+          <t>17:32</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
@@ -2646,7 +2646,7 @@
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>17:29</t>
+          <t>17:32</t>
         </is>
       </c>
       <c r="E89" t="inlineStr">
@@ -2666,17 +2666,17 @@
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>5,03</t>
+          <t>4,93</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>22:32</t>
+          <t>17:29</t>
         </is>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t xml:space="preserve"> quarta-feira, 5 de abril de 2023 </t>
+          <t xml:space="preserve"> quinta-feira, 13 de abril de 2023 </t>
         </is>
       </c>
     </row>
@@ -2691,17 +2691,17 @@
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>5,48</t>
+          <t>5,44</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>22:32</t>
+          <t>17:29</t>
         </is>
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t xml:space="preserve"> quarta-feira, 5 de abril de 2023 </t>
+          <t xml:space="preserve"> quinta-feira, 13 de abril de 2023 </t>
         </is>
       </c>
     </row>
@@ -2716,17 +2716,17 @@
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>0,038</t>
+          <t>0,037</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>22:32</t>
+          <t>17:29</t>
         </is>
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t xml:space="preserve"> quarta-feira, 5 de abril de 2023 </t>
+          <t xml:space="preserve"> quinta-feira, 13 de abril de 2023 </t>
         </is>
       </c>
     </row>
@@ -2741,17 +2741,17 @@
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>0,73</t>
+          <t>0,72</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>22:32</t>
+          <t>17:29</t>
         </is>
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t xml:space="preserve"> quarta-feira, 5 de abril de 2023 </t>
+          <t xml:space="preserve"> quinta-feira, 13 de abril de 2023 </t>
         </is>
       </c>
     </row>
@@ -2771,7 +2771,7 @@
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>21:21</t>
+          <t>22:32</t>
         </is>
       </c>
       <c r="E94" t="inlineStr">
@@ -2791,12 +2791,12 @@
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>5,49</t>
+          <t>5,48</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>21:21</t>
+          <t>22:32</t>
         </is>
       </c>
       <c r="E95" t="inlineStr">
@@ -2821,7 +2821,7 @@
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>21:21</t>
+          <t>22:32</t>
         </is>
       </c>
       <c r="E96" t="inlineStr">
@@ -2846,7 +2846,7 @@
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>21:21</t>
+          <t>22:32</t>
         </is>
       </c>
       <c r="E97" t="inlineStr">
@@ -2871,7 +2871,7 @@
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>21:20</t>
+          <t>21:21</t>
         </is>
       </c>
       <c r="E98" t="inlineStr">
@@ -2896,7 +2896,7 @@
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>21:20</t>
+          <t>21:21</t>
         </is>
       </c>
       <c r="E99" t="inlineStr">
@@ -2921,7 +2921,7 @@
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>21:20</t>
+          <t>21:21</t>
         </is>
       </c>
       <c r="E100" t="inlineStr">
@@ -2946,7 +2946,7 @@
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>21:20</t>
+          <t>21:21</t>
         </is>
       </c>
       <c r="E101" t="inlineStr">
@@ -3050,6 +3050,106 @@
         </is>
       </c>
       <c r="E105" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> quarta-feira, 5 de abril de 2023 </t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" s="1" t="n">
+        <v>104</v>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>Dollar</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>5,03</t>
+        </is>
+      </c>
+      <c r="D106" t="inlineStr">
+        <is>
+          <t>21:20</t>
+        </is>
+      </c>
+      <c r="E106" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> quarta-feira, 5 de abril de 2023 </t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" s="1" t="n">
+        <v>105</v>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>Euro</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>5,49</t>
+        </is>
+      </c>
+      <c r="D107" t="inlineStr">
+        <is>
+          <t>21:20</t>
+        </is>
+      </c>
+      <c r="E107" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> quarta-feira, 5 de abril de 2023 </t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" s="1" t="n">
+        <v>106</v>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>Iene</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>0,038</t>
+        </is>
+      </c>
+      <c r="D108" t="inlineStr">
+        <is>
+          <t>21:20</t>
+        </is>
+      </c>
+      <c r="E108" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> quarta-feira, 5 de abril de 2023 </t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" s="1" t="n">
+        <v>107</v>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>Yuan Chinês</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>0,73</t>
+        </is>
+      </c>
+      <c r="D109" t="inlineStr">
+        <is>
+          <t>21:20</t>
+        </is>
+      </c>
+      <c r="E109" t="inlineStr">
         <is>
           <t xml:space="preserve"> quarta-feira, 5 de abril de 2023 </t>
         </is>

</xml_diff>